<commit_message>
Fallos altura poligono e if altura final
</commit_message>
<xml_diff>
--- a/Matlab/Shapes.xlsx
+++ b/Matlab/Shapes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upm365-my.sharepoint.com/personal/daniel_delrio_velilla_alumnos_upm_es/Documents/MUSE/S3/TeP/Mecanizado/Automatic_gcode_Generator/Matlab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="11_AD4D2F04E46CFB4ACB3E20C29552CDFC693EDF15" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0684092-0873-439E-8448-D5AC4EE8D8D4}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="11_AD4D2F04E46CFB4ACB3E20C29552CDFC693EDF15" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C67A28E9-E1B2-474C-8E84-BE487898BEB2}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1800" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3405" yWindow="4365" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -377,7 +377,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,10 +431,10 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -465,11 +465,14 @@
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="E5" s="2">
-        <v>-20</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>

</xml_diff>

<commit_message>
Corregido fallo  pasadas funales + limpiar codigo
</commit_message>
<xml_diff>
--- a/Matlab/Shapes.xlsx
+++ b/Matlab/Shapes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upm365-my.sharepoint.com/personal/daniel_delrio_velilla_alumnos_upm_es/Documents/MUSE/S3/TeP/Mecanizado/Automatic_gcode_Generator/Matlab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="270" documentId="11_AD4D2F04E46CFB4ACB3E20C29552CDFC693EDF15" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3483EBD-93E0-4EF2-B36F-69F9BABBA940}"/>
+  <xr:revisionPtr revIDLastSave="278" documentId="11_AD4D2F04E46CFB4ACB3E20C29552CDFC693EDF15" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57E65347-3153-4C07-8D99-008D3AAFE16A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3690" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="990" yWindow="4365" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE2EFDA"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -111,13 +111,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Énfasis3" xfId="1" builtinId="38"/>
@@ -402,7 +399,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A2" sqref="A2:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,195 +429,195 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2" s="2">
         <v>6</v>
       </c>
-      <c r="B2" s="4">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="2">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
         <v>14.33</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>6.5</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="2">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4">
+      <c r="A3" s="2">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
         <v>5.75</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <v>25</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="2">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>35.659999999999997</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43.5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>14.33</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>34.25</v>
+      </c>
+      <c r="D6" s="2">
+        <v>15.75</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="C8" s="2">
+        <v>15.75</v>
+      </c>
+      <c r="D8" s="2">
+        <v>15.75</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>14.33</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2">
+        <v>5.75</v>
+      </c>
+      <c r="C10" s="2">
         <v>5.4569999999999999</v>
       </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4">
-        <v>35.659999999999997</v>
-      </c>
-      <c r="D4" s="4">
-        <v>6.5</v>
-      </c>
-      <c r="E4" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4">
-        <v>5</v>
-      </c>
-      <c r="C5" s="4">
-        <v>43.5</v>
-      </c>
-      <c r="D5" s="4">
-        <v>14.33</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4">
-        <v>5.5</v>
-      </c>
-      <c r="C6" s="4">
-        <v>34.25</v>
-      </c>
-      <c r="D6" s="4">
-        <v>15.75</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>0</v>
-      </c>
-      <c r="B7" s="4">
+      <c r="D10" s="2">
+        <v>25</v>
+      </c>
+      <c r="E10" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2">
         <v>10</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C11" s="2">
+        <v>16.867999999999999</v>
+      </c>
+      <c r="D11" s="2">
         <v>25</v>
       </c>
-      <c r="D7" s="5">
-        <v>16.867999999999999</v>
-      </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>4</v>
-      </c>
-      <c r="B8" s="4">
-        <v>5.5</v>
-      </c>
-      <c r="C8" s="4">
-        <v>15.75</v>
-      </c>
-      <c r="D8" s="4">
-        <v>15.75</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4">
-        <v>5</v>
-      </c>
-      <c r="C9" s="4">
-        <v>6.5</v>
-      </c>
-      <c r="D9" s="4">
-        <v>14.33</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>5</v>
-      </c>
-      <c r="B10" s="4">
-        <v>5.75</v>
-      </c>
-      <c r="C10" s="4">
-        <v>5.4569999999999999</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2">
+        <v>33</v>
+      </c>
+      <c r="D12" s="2">
         <v>25</v>
       </c>
-      <c r="E10" s="4">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>0</v>
-      </c>
-      <c r="B11" s="4">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4">
-        <v>16.867999999999999</v>
-      </c>
-      <c r="D11" s="4">
-        <v>25</v>
-      </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>0</v>
-      </c>
-      <c r="B12" s="4">
-        <v>10</v>
-      </c>
-      <c r="C12" s="5">
-        <v>33.131999999999998</v>
-      </c>
-      <c r="D12" s="4">
-        <v>25</v>
-      </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>5</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="2">
         <v>5.75</v>
       </c>
-      <c r="C13" s="3">
-        <v>44.542999999999999</v>
+      <c r="C13" s="2">
+        <v>45</v>
       </c>
       <c r="D13" s="2">
         <v>25</v>
@@ -630,136 +627,136 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="2">
         <v>6</v>
       </c>
-      <c r="B14" s="4">
-        <v>5</v>
-      </c>
-      <c r="C14" s="4">
+      <c r="B14" s="2">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2">
         <v>43.5</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="2">
         <v>35.67</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="2">
         <v>4</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="2">
         <v>5.5</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="2">
         <v>34.25</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="2">
         <v>34.25</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>0</v>
-      </c>
-      <c r="B16" s="4">
+      <c r="A16" s="2">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2">
         <v>10</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="2">
         <v>25</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="2">
         <v>33.131999999999998</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="2">
         <v>4</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="2">
         <v>5.5</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="2">
         <v>15.75</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="2">
         <v>34.25</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18" s="2">
         <v>6</v>
       </c>
-      <c r="B18" s="4">
-        <v>5</v>
-      </c>
-      <c r="C18" s="4">
+      <c r="B18" s="2">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2">
         <v>6.5</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="2">
         <v>35.67</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19" s="2">
         <v>6</v>
       </c>
-      <c r="B19" s="4">
-        <v>5</v>
-      </c>
-      <c r="C19" s="4">
+      <c r="B19" s="2">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2">
         <v>14.33</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="2">
         <v>43.5</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="2">
         <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>5</v>
-      </c>
-      <c r="B20" s="4">
+      <c r="A20" s="2">
+        <v>5</v>
+      </c>
+      <c r="B20" s="2">
         <v>5.75</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="2">
         <v>25</v>
       </c>
-      <c r="D20" s="5">
-        <v>44.542999999999999</v>
-      </c>
-      <c r="E20" s="4">
+      <c r="D20" s="2">
+        <v>45</v>
+      </c>
+      <c r="E20" s="2">
         <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="A21" s="2">
         <v>6</v>
       </c>
-      <c r="B21" s="4">
-        <v>5</v>
-      </c>
-      <c r="C21" s="4">
+      <c r="B21" s="2">
+        <v>5</v>
+      </c>
+      <c r="C21" s="2">
         <v>35.67</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="2">
         <v>43.5</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="2">
         <v>30</v>
       </c>
     </row>

</xml_diff>